<commit_message>
Transaktionen ausprogrammiert RSA Verschlüsselung begonnen
</commit_message>
<xml_diff>
--- a/Testprotokoll.xlsx
+++ b/Testprotokoll.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DiagnosticChain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58D2ABE-6D0C-4A27-9603-98382ADC227B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B9C709-3F66-4F8D-83E7-45390E69DDE3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Neue Transaktionen generieren</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>JSON-Repräsentationen austesten</t>
+  </si>
+  <si>
+    <t>Transaktionen korrekt verschlüsseln</t>
   </si>
 </sst>
 </file>
@@ -112,12 +115,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -132,11 +141,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -417,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,123 +438,132 @@
     <col min="1" max="1" width="58.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>